<commit_message>
Imported msidata and msiuniv files. Starting to create tables for Affiliation section.
</commit_message>
<xml_diff>
--- a/tables/UnivIndex.xlsx
+++ b/tables/UnivIndex.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1147" documentId="13_ncr:40009_{693690F3-2ABB-4F24-AAC9-1084920C2D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C386DB24-4A7C-478D-AF4D-61D5CBCF6002}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="45" windowWidth="24420" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1035" windowWidth="15870" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnivIndex" sheetId="1" r:id="rId1"/>
@@ -4230,7 +4230,7 @@
       <sheetName val="Just Program Eligibility"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
+      <sheetData sheetId="0">
         <row r="1">
           <cell r="B1"/>
         </row>
@@ -42061,7 +42061,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
Created Network Analysis Rmd. Removed sections for SNA, University Collaborations, DCA. Revised DraftUnivList.xlsx
</commit_message>
<xml_diff>
--- a/tables/UnivIndex.xlsx
+++ b/tables/UnivIndex.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1147" documentId="13_ncr:40009_{693690F3-2ABB-4F24-AAC9-1084920C2D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C386DB24-4A7C-478D-AF4D-61D5CBCF6002}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1035" windowWidth="15870" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10890" yWindow="435" windowWidth="24660" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnivIndex" sheetId="1" r:id="rId1"/>
@@ -4231,39 +4231,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1"/>
-        </row>
-        <row r="2">
-          <cell r="B2"/>
-        </row>
-        <row r="3">
-          <cell r="B3"/>
-        </row>
-        <row r="4">
-          <cell r="B4"/>
-        </row>
-        <row r="5">
-          <cell r="B5"/>
-        </row>
-        <row r="6">
-          <cell r="B6"/>
-        </row>
-        <row r="7">
-          <cell r="B7"/>
-        </row>
-        <row r="8">
-          <cell r="B8"/>
-        </row>
-        <row r="9">
-          <cell r="B9"/>
-        </row>
-        <row r="10">
-          <cell r="B10"/>
-        </row>
-        <row r="11">
-          <cell r="B11"/>
-        </row>
         <row r="12">
           <cell r="A12" t="str">
             <v>Institution Name</v>
@@ -42366,7 +42333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F662"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B466" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B642" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C483" sqref="C483"/>
     </sheetView>
   </sheetViews>

</xml_diff>